<commit_message>
updated condition of Display mode button on EBOM page to work through Jenkins
</commit_message>
<xml_diff>
--- a/Enovia-3DExperience/src/test/resources/Repository.xlsx
+++ b/Enovia-3DExperience/src/test/resources/Repository.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="261">
   <si>
     <t>Type</t>
   </si>
@@ -821,6 +821,9 @@
   </si>
   <si>
     <t>Part-48851417-0000389-01</t>
+  </si>
+  <si>
+    <t>Part-48851417-0000394-01</t>
   </si>
 </sst>
 </file>
@@ -1864,7 +1867,7 @@
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
updated display mode icon visibility logic on ebom page
</commit_message>
<xml_diff>
--- a/Enovia-3DExperience/src/test/resources/Repository.xlsx
+++ b/Enovia-3DExperience/src/test/resources/Repository.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="262">
   <si>
     <t>Type</t>
   </si>
@@ -824,6 +824,9 @@
   </si>
   <si>
     <t>Part-48851417-0000394-01</t>
+  </si>
+  <si>
+    <t>Part-48851417-0000398-01</t>
   </si>
 </sst>
 </file>
@@ -1867,7 +1870,7 @@
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Updated Feature file and task link click logic
</commit_message>
<xml_diff>
--- a/Enovia-3DExperience/src/test/resources/Repository.xlsx
+++ b/Enovia-3DExperience/src/test/resources/Repository.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="267">
   <si>
     <t>Type</t>
   </si>
@@ -827,6 +827,21 @@
   </si>
   <si>
     <t>Part-48851417-0000398-01</t>
+  </si>
+  <si>
+    <t>Part-48851417-0000399-01</t>
+  </si>
+  <si>
+    <t>Part-48851417-0000400-01</t>
+  </si>
+  <si>
+    <t>Part-48851417-0000402-01</t>
+  </si>
+  <si>
+    <t>Part-48851417-0000404-01</t>
+  </si>
+  <si>
+    <t>Part-48851417-0000406-01</t>
   </si>
 </sst>
 </file>
@@ -1870,7 +1885,7 @@
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3">

</xml_diff>